<commit_message>
Added cross browser functionality
</commit_message>
<xml_diff>
--- a/target/test-classes/com/ar/testdata/ValidateAR.xlsx
+++ b/target/test-classes/com/ar/testdata/ValidateAR.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB22F9BD-CB39-4375-8E47-16B91A41274F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9D434D-CC23-402C-BB02-009E01284E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
-  <si>
-    <t>venkat</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>p</t>
   </si>
@@ -44,6 +41,18 @@
   </si>
   <si>
     <t>(UTC+00:00:00) Atlantic/Canary</t>
+  </si>
+  <si>
+    <t>venkat1</t>
+  </si>
+  <si>
+    <t>venkat2</t>
+  </si>
+  <si>
+    <t>venkat3</t>
+  </si>
+  <si>
+    <t>venkat4</t>
   </si>
 </sst>
 </file>
@@ -398,7 +407,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,82 +422,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
       <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>